<commit_message>
I made the changes
</commit_message>
<xml_diff>
--- a/Expenses01.xlsx
+++ b/Expenses01.xlsx
@@ -349,87 +349,87 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D1">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E1">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>19</v>
+      </c>
+      <c r="C2">
+        <v>22</v>
+      </c>
+      <c r="D2">
+        <v>13</v>
+      </c>
+      <c r="E2">
         <v>23</v>
-      </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>14</v>
-      </c>
-      <c r="D2">
-        <v>9</v>
-      </c>
-      <c r="E2">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B3">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>16</v>
       </c>
       <c r="D3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E3">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B4">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D4">
+        <v>23</v>
+      </c>
+      <c r="E4">
         <v>4</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C5">
         <v>18</v>
       </c>
       <c r="D5">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E5">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>